<commit_message>
Admin funcionalidad, vehiculos clientes, etc
</commit_message>
<xml_diff>
--- a/AutoFixProyectoWeb/AutoFixProyectoWeb/Plantillas/plantilla_factura.xlsx
+++ b/AutoFixProyectoWeb/AutoFixProyectoWeb/Plantillas/plantilla_factura.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Freelance\Projects\Esteban 2024\06-08-2024\Proyecto-EstacionDeServicio\AutoFixProyectoWeb\AutoFixProyectoWeb\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Freelance\Projects\Esteban 2024\17-08-2024\Proyecto-EstacionDeServicio\AutoFixProyectoWeb\AutoFixProyectoWeb\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEBA1D5-4ABB-4D5F-B01F-57A25A4DA785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C553C9-FCF4-46DF-9E96-CCF965147A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87EB77F6-4453-4E25-A7DC-10897C9CA807}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FACTURA</t>
   </si>
   <si>
-    <t>Servicio</t>
-  </si>
-  <si>
     <t>Descripcion</t>
   </si>
   <si>
@@ -55,6 +52,12 @@
   </si>
   <si>
     <t>Total a pagar:</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -140,17 +143,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,12 +518,12 @@
   <dimension ref="A4:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E36"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
@@ -531,28 +531,28 @@
   <sheetData>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="9"/>
       <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="9"/>
+      <c r="E6" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D6" s="7"/>
-      <c r="E6" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -560,15 +560,15 @@
       <c r="C7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
@@ -576,75 +576,77 @@
     </row>
     <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="4" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
@@ -687,25 +689,9 @@
       <c r="E36" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="2">
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="D4:D8"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>